<commit_message>
actualizar listas desde un archivo
</commit_message>
<xml_diff>
--- a/bd/alumnos2018.xlsx
+++ b/bd/alumnos2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marifer\Documents\NetBeansProjects\TutoriasUnsis\bd\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mine\Documents\TutoriasSS\TutoriasUnsis\bd\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>matricula</t>
   </si>
@@ -32,37 +32,31 @@
     <t>nombre</t>
   </si>
   <si>
-    <t>apellidoP</t>
-  </si>
-  <si>
-    <t>apellidoM</t>
-  </si>
-  <si>
-    <t>Perez</t>
-  </si>
-  <si>
     <t>Maribel</t>
   </si>
   <si>
-    <t>Ramirez</t>
-  </si>
-  <si>
-    <t>Sanchez</t>
-  </si>
-  <si>
-    <t>2018060124</t>
-  </si>
-  <si>
     <t>pancracia</t>
   </si>
   <si>
-    <t>2015060149</t>
+    <t>grupo</t>
+  </si>
+  <si>
+    <t>906-a</t>
+  </si>
+  <si>
+    <t>2018060161</t>
+  </si>
+  <si>
+    <t>806-b</t>
+  </si>
+  <si>
+    <t>2015060162</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -107,7 +101,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,7 +382,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -396,11 +390,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="11.42578125" style="1"/>
-    <col min="5" max="6" width="11.42578125" style="5"/>
+    <col min="1" max="3" width="11.42578125" style="1"/>
+    <col min="4" max="4" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -408,61 +402,49 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4">
-        <v>1</v>
-      </c>
-      <c r="F1" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="4">
-        <v>906</v>
-      </c>
-      <c r="F2" s="6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="4">
-        <v>806</v>
-      </c>
-      <c r="F3" s="4">
-        <v>6</v>
-      </c>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H12" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F9" s="6"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F12" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>